<commit_message>
changed period_ID and er diagram
</commit_message>
<xml_diff>
--- a/Data/Item_Period_data.xlsx
+++ b/Data/Item_Period_data.xlsx
@@ -19,7 +19,7 @@
     <t>Item_ID</t>
   </si>
   <si>
-    <t>Period</t>
+    <t>Period_ID</t>
   </si>
   <si>
     <t>Gross_Requirement</t>
@@ -42,7 +42,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +53,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -86,13 +92,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -441,7 +447,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -458,7 +464,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -475,7 +481,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -492,7 +498,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -509,7 +515,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -526,7 +532,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3">
         <v>2</v>
       </c>
@@ -543,7 +549,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3">
         <v>2</v>
       </c>
@@ -560,7 +566,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -577,7 +583,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3">
         <v>2</v>
       </c>
@@ -594,7 +600,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3">
         <v>2</v>
       </c>

</xml_diff>